<commit_message>
dev D_BIT <-> A_BIT
</commit_message>
<xml_diff>
--- a/docs/5stage_fht64.xlsx
+++ b/docs/5stage_fht64.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SS\fpga\fft\fht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpga\fht\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -334,6 +334,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -614,15 +620,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10:S12"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="9.140625" style="26"/>
+    <col min="13" max="13" width="9.140625" style="25"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +657,7 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="26" t="s">
         <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -659,7 +669,7 @@
       <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="N1" t="s">
@@ -669,7 +679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -696,7 +706,7 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="26">
         <v>2</v>
       </c>
       <c r="J2" s="4">
@@ -706,10 +716,10 @@
         <v>2.4</v>
       </c>
       <c r="L2" s="6">
-        <v>1</v>
-      </c>
-      <c r="M2" t="str">
-        <f>DEC2BIN(D2,5)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="25" t="str">
+        <f t="shared" ref="M2:M33" si="0">DEC2BIN(D2,5)</f>
         <v>00000</v>
       </c>
       <c r="N2" s="24">
@@ -720,28 +730,13 @@
         <f>BIN2DEC(N2)</f>
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="str">
-        <f>DEC2BIN(P2,4)</f>
-        <v>0000</v>
-      </c>
-      <c r="R2">
-        <f>SUMPRODUCT(MID($Q2,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <f>BIN2DEC(R2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <f t="shared" ref="B3:B4" si="0">A3+1</f>
+        <f t="shared" ref="B3:B4" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="C3" s="5">
@@ -754,7 +749,7 @@
         <v>32</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F33" si="1">E3+1</f>
+        <f t="shared" ref="F3:F33" si="2">E3+1</f>
         <v>33</v>
       </c>
       <c r="G3">
@@ -770,10 +765,10 @@
         <v>3.1</v>
       </c>
       <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" t="str">
-        <f>DEC2BIN(D3,5)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="N3" s="24">
@@ -781,31 +776,16 @@
         <v>1</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O33" si="2">BIN2DEC(N3)</f>
+        <f t="shared" ref="O3:O33" si="3">BIN2DEC(N3)</f>
         <v>1</v>
       </c>
-      <c r="P3">
-        <v>8</v>
-      </c>
-      <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q8" si="3">DEC2BIN(P3,4)</f>
-        <v>1000</v>
-      </c>
-      <c r="R3">
-        <f>SUMPRODUCT(MID($Q3,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S8" si="4">BIN2DEC(R3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>4</v>
       </c>
       <c r="B4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C4" s="5">
@@ -818,7 +798,7 @@
         <v>16</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G4">
@@ -827,7 +807,7 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="26">
         <v>2</v>
       </c>
       <c r="J4" s="14">
@@ -839,8 +819,8 @@
       <c r="L4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M4" t="str">
-        <f>DEC2BIN(D4,5)</f>
+      <c r="M4" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01000</v>
       </c>
       <c r="N4" s="24">
@@ -848,31 +828,16 @@
         <v>10</v>
       </c>
       <c r="O4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="P4">
-        <v>4</v>
-      </c>
-      <c r="Q4" t="str">
-        <f t="shared" si="3"/>
-        <v>0100</v>
-      </c>
-      <c r="R4">
-        <f>SUMPRODUCT(MID($Q4,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>10</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>6</v>
       </c>
       <c r="B5" s="5">
-        <f t="shared" ref="B5:B33" si="5">A5+1</f>
+        <f t="shared" ref="B5:B33" si="4">A5+1</f>
         <v>7</v>
       </c>
       <c r="C5" s="5">
@@ -885,7 +850,7 @@
         <v>48</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="G5">
@@ -903,8 +868,8 @@
       <c r="L5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="M5" t="str">
-        <f>DEC2BIN(D5,5)</f>
+      <c r="M5" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11000</v>
       </c>
       <c r="N5" s="24">
@@ -912,31 +877,16 @@
         <v>11</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="P5">
-        <v>12</v>
-      </c>
-      <c r="Q5" t="str">
-        <f t="shared" si="3"/>
-        <v>1100</v>
-      </c>
-      <c r="R5">
-        <f>SUMPRODUCT(MID($Q5,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>11</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>8</v>
       </c>
       <c r="B6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="C6" s="5">
@@ -949,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G6">
@@ -958,7 +908,7 @@
       <c r="H6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="26">
         <v>4</v>
       </c>
       <c r="J6" s="14">
@@ -970,8 +920,8 @@
       <c r="L6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M6" t="str">
-        <f>DEC2BIN(D6,5)</f>
+      <c r="M6" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00100</v>
       </c>
       <c r="N6" s="24">
@@ -979,31 +929,16 @@
         <v>100</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P6">
-        <v>2</v>
-      </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="3"/>
-        <v>0010</v>
-      </c>
-      <c r="R6">
-        <f>SUMPRODUCT(MID($Q6,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>100</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>10</v>
       </c>
       <c r="B7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="C7" s="5">
@@ -1016,7 +951,7 @@
         <v>40</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="G7">
@@ -1034,8 +969,8 @@
       <c r="L7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M7" t="str">
-        <f>DEC2BIN(D7,5)</f>
+      <c r="M7" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10100</v>
       </c>
       <c r="N7" s="24">
@@ -1043,31 +978,16 @@
         <v>101</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
-      <c r="Q7" t="str">
-        <f t="shared" si="3"/>
-        <v>1010</v>
-      </c>
-      <c r="R7">
-        <f>SUMPRODUCT(MID($Q7,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>101</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>12</v>
       </c>
       <c r="B8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="C8" s="5">
@@ -1080,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="G8">
@@ -1098,8 +1018,8 @@
       <c r="L8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M8" t="str">
-        <f>DEC2BIN(D8,5)</f>
+      <c r="M8" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01100</v>
       </c>
       <c r="N8" s="24">
@@ -1107,31 +1027,16 @@
         <v>110</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P8">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="3"/>
-        <v>0110</v>
-      </c>
-      <c r="R8">
-        <f>SUMPRODUCT(MID($Q8,{1;2;3;4},1)*10^{0;1;2;3})</f>
-        <v>110</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>14</v>
       </c>
       <c r="B9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="C9" s="5">
@@ -1144,7 +1049,7 @@
         <v>56</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="G9">
@@ -1162,8 +1067,8 @@
       <c r="L9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M9" t="str">
-        <f>DEC2BIN(D9,5)</f>
+      <c r="M9" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11100</v>
       </c>
       <c r="N9" s="24">
@@ -1171,16 +1076,16 @@
         <v>111</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>16</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="C10" s="5">
@@ -1193,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G10">
@@ -1202,7 +1107,7 @@
       <c r="H10">
         <v>8</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="26">
         <v>8</v>
       </c>
       <c r="J10" s="14">
@@ -1214,8 +1119,8 @@
       <c r="L10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M10" t="str">
-        <f>DEC2BIN(D10,5)</f>
+      <c r="M10" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00010</v>
       </c>
       <c r="N10" s="24">
@@ -1223,16 +1128,16 @@
         <v>1000</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="C11" s="5">
@@ -1245,7 +1150,7 @@
         <v>36</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="G11">
@@ -1263,8 +1168,8 @@
       <c r="L11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M11" t="str">
-        <f>DEC2BIN(D11,5)</f>
+      <c r="M11" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10010</v>
       </c>
       <c r="N11" s="24">
@@ -1272,16 +1177,16 @@
         <v>1001</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>20</v>
       </c>
       <c r="B12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="C12" s="5">
@@ -1294,7 +1199,7 @@
         <v>20</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="G12">
@@ -1312,8 +1217,8 @@
       <c r="L12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M12" t="str">
-        <f>DEC2BIN(D12,5)</f>
+      <c r="M12" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01010</v>
       </c>
       <c r="N12" s="24">
@@ -1321,16 +1226,16 @@
         <v>1010</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>22</v>
       </c>
       <c r="B13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="C13" s="5">
@@ -1343,7 +1248,7 @@
         <v>52</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="G13">
@@ -1361,8 +1266,8 @@
       <c r="L13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M13" t="str">
-        <f>DEC2BIN(D13,5)</f>
+      <c r="M13" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11010</v>
       </c>
       <c r="N13" s="24">
@@ -1370,16 +1275,16 @@
         <v>1011</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>24</v>
       </c>
       <c r="B14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="C14" s="5">
@@ -1392,7 +1297,7 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G14">
@@ -1410,8 +1315,8 @@
       <c r="L14" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M14" t="str">
-        <f>DEC2BIN(D14,5)</f>
+      <c r="M14" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00110</v>
       </c>
       <c r="N14" s="24">
@@ -1419,16 +1324,16 @@
         <v>1100</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>26</v>
       </c>
       <c r="B15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="C15" s="5">
@@ -1441,7 +1346,7 @@
         <v>44</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="G15">
@@ -1459,8 +1364,8 @@
       <c r="L15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M15" t="str">
-        <f>DEC2BIN(D15,5)</f>
+      <c r="M15" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10110</v>
       </c>
       <c r="N15" s="24">
@@ -1468,16 +1373,16 @@
         <v>1101</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>28</v>
       </c>
       <c r="B16" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="C16" s="5">
@@ -1490,7 +1395,7 @@
         <v>28</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="G16">
@@ -1508,8 +1413,8 @@
       <c r="L16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M16" t="str">
-        <f>DEC2BIN(D16,5)</f>
+      <c r="M16" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01110</v>
       </c>
       <c r="N16" s="24">
@@ -1517,7 +1422,7 @@
         <v>1110</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
@@ -1526,7 +1431,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="C17" s="5">
@@ -1539,7 +1444,7 @@
         <v>60</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="G17">
@@ -1557,8 +1462,8 @@
       <c r="L17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M17" t="str">
-        <f>DEC2BIN(D17,5)</f>
+      <c r="M17" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11110</v>
       </c>
       <c r="N17" s="24">
@@ -1566,7 +1471,7 @@
         <v>1111</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -1575,7 +1480,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="C18" s="5">
@@ -1588,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G18">
@@ -1597,7 +1502,7 @@
       <c r="H18">
         <v>16</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="26">
         <v>16</v>
       </c>
       <c r="J18" s="21">
@@ -1607,8 +1512,8 @@
       <c r="L18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="M18" t="str">
-        <f>DEC2BIN(D18,5)</f>
+      <c r="M18" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00001</v>
       </c>
       <c r="N18" s="24">
@@ -1616,7 +1521,7 @@
         <v>10000</v>
       </c>
       <c r="O18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
@@ -1625,7 +1530,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="C19" s="5">
@@ -1638,7 +1543,7 @@
         <v>34</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="G19">
@@ -1654,8 +1559,8 @@
       <c r="L19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M19" t="str">
-        <f>DEC2BIN(D19,5)</f>
+      <c r="M19" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10001</v>
       </c>
       <c r="N19" s="24">
@@ -1663,7 +1568,7 @@
         <v>10001</v>
       </c>
       <c r="O19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
     </row>
@@ -1672,7 +1577,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="C20" s="5">
@@ -1685,7 +1590,7 @@
         <v>18</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="G20">
@@ -1701,8 +1606,8 @@
       <c r="L20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M20" t="str">
-        <f>DEC2BIN(D20,5)</f>
+      <c r="M20" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01001</v>
       </c>
       <c r="N20" s="24">
@@ -1710,7 +1615,7 @@
         <v>10010</v>
       </c>
       <c r="O20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
@@ -1719,7 +1624,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="C21" s="5">
@@ -1732,7 +1637,7 @@
         <v>50</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="G21">
@@ -1748,8 +1653,8 @@
       <c r="L21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M21" t="str">
-        <f>DEC2BIN(D21,5)</f>
+      <c r="M21" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11001</v>
       </c>
       <c r="N21" s="24">
@@ -1757,7 +1662,7 @@
         <v>10011</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
@@ -1766,7 +1671,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="C22" s="5">
@@ -1779,7 +1684,7 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G22">
@@ -1795,8 +1700,8 @@
       <c r="L22" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M22" t="str">
-        <f>DEC2BIN(D22,5)</f>
+      <c r="M22" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00101</v>
       </c>
       <c r="N22" s="24">
@@ -1804,7 +1709,7 @@
         <v>10100</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -1813,7 +1718,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="C23" s="5">
@@ -1826,7 +1731,7 @@
         <v>42</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="G23">
@@ -1842,8 +1747,8 @@
       <c r="L23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M23" t="str">
-        <f>DEC2BIN(D23,5)</f>
+      <c r="M23" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10101</v>
       </c>
       <c r="N23" s="24">
@@ -1851,7 +1756,7 @@
         <v>10101</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
     </row>
@@ -1860,7 +1765,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="C24" s="5">
@@ -1873,7 +1778,7 @@
         <v>26</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="G24">
@@ -1889,8 +1794,8 @@
       <c r="L24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M24" t="str">
-        <f>DEC2BIN(D24,5)</f>
+      <c r="M24" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01101</v>
       </c>
       <c r="N24" s="24">
@@ -1898,7 +1803,7 @@
         <v>10110</v>
       </c>
       <c r="O24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
     </row>
@@ -1907,7 +1812,7 @@
         <v>46</v>
       </c>
       <c r="B25" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="C25" s="5">
@@ -1920,7 +1825,7 @@
         <v>58</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="G25">
@@ -1936,8 +1841,8 @@
       <c r="L25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M25" t="str">
-        <f>DEC2BIN(D25,5)</f>
+      <c r="M25" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11101</v>
       </c>
       <c r="N25" s="24">
@@ -1945,7 +1850,7 @@
         <v>10111</v>
       </c>
       <c r="O25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
@@ -1954,7 +1859,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="C26" s="5">
@@ -1967,7 +1872,7 @@
         <v>6</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G26">
@@ -1983,8 +1888,8 @@
       <c r="L26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M26" t="str">
-        <f>DEC2BIN(D26,5)</f>
+      <c r="M26" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00011</v>
       </c>
       <c r="N26" s="24">
@@ -1992,7 +1897,7 @@
         <v>11000</v>
       </c>
       <c r="O26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
     </row>
@@ -2001,7 +1906,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="C27" s="5">
@@ -2014,7 +1919,7 @@
         <v>38</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="G27">
@@ -2030,8 +1935,8 @@
       <c r="L27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M27" t="str">
-        <f>DEC2BIN(D27,5)</f>
+      <c r="M27" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10011</v>
       </c>
       <c r="N27" s="24">
@@ -2039,7 +1944,7 @@
         <v>11001</v>
       </c>
       <c r="O27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
@@ -2048,7 +1953,7 @@
         <v>52</v>
       </c>
       <c r="B28" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="C28" s="5">
@@ -2061,7 +1966,7 @@
         <v>22</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="G28">
@@ -2070,8 +1975,8 @@
       <c r="H28">
         <v>26</v>
       </c>
-      <c r="M28" t="str">
-        <f>DEC2BIN(D28,5)</f>
+      <c r="M28" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01011</v>
       </c>
       <c r="N28" s="24">
@@ -2079,7 +1984,7 @@
         <v>11010</v>
       </c>
       <c r="O28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
     </row>
@@ -2088,7 +1993,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="C29" s="5">
@@ -2101,7 +2006,7 @@
         <v>54</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="G29">
@@ -2110,8 +2015,8 @@
       <c r="H29">
         <v>27</v>
       </c>
-      <c r="M29" t="str">
-        <f>DEC2BIN(D29,5)</f>
+      <c r="M29" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11011</v>
       </c>
       <c r="N29" s="24">
@@ -2119,7 +2024,7 @@
         <v>11011</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
@@ -2128,7 +2033,7 @@
         <v>56</v>
       </c>
       <c r="B30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="C30" s="5">
@@ -2141,7 +2046,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G30">
@@ -2150,8 +2055,8 @@
       <c r="H30">
         <v>28</v>
       </c>
-      <c r="M30" t="str">
-        <f>DEC2BIN(D30,5)</f>
+      <c r="M30" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>00111</v>
       </c>
       <c r="N30" s="24">
@@ -2159,7 +2064,7 @@
         <v>11100</v>
       </c>
       <c r="O30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
     </row>
@@ -2168,7 +2073,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="C31" s="5">
@@ -2181,7 +2086,7 @@
         <v>46</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="G31">
@@ -2190,8 +2095,8 @@
       <c r="H31">
         <v>29</v>
       </c>
-      <c r="M31" t="str">
-        <f>DEC2BIN(D31,5)</f>
+      <c r="M31" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>10111</v>
       </c>
       <c r="N31" s="24">
@@ -2199,7 +2104,7 @@
         <v>11101</v>
       </c>
       <c r="O31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
     </row>
@@ -2208,7 +2113,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="C32" s="5">
@@ -2221,7 +2126,7 @@
         <v>30</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="G32">
@@ -2230,8 +2135,8 @@
       <c r="H32">
         <v>30</v>
       </c>
-      <c r="M32" t="str">
-        <f>DEC2BIN(D32,5)</f>
+      <c r="M32" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>01111</v>
       </c>
       <c r="N32" s="24">
@@ -2239,7 +2144,7 @@
         <v>11110</v>
       </c>
       <c r="O32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
@@ -2248,7 +2153,7 @@
         <v>62</v>
       </c>
       <c r="B33" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="C33" s="8">
@@ -2261,7 +2166,7 @@
         <v>62</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="G33">
@@ -2270,8 +2175,8 @@
       <c r="H33">
         <v>31</v>
       </c>
-      <c r="M33" t="str">
-        <f>DEC2BIN(D33,5)</f>
+      <c r="M33" s="25" t="str">
+        <f t="shared" si="0"/>
         <v>11111</v>
       </c>
       <c r="N33" s="24">
@@ -2279,7 +2184,7 @@
         <v>11111</v>
       </c>
       <c r="O33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
     </row>

</xml_diff>